<commit_message>
Add apply, and update survey
</commit_message>
<xml_diff>
--- a/r-fundamentals-5/data/tflSubset.xlsx
+++ b/r-fundamentals-5/data/tflSubset.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2259,6 +2259,32 @@
         <v>6.5</v>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>03_21/22</t>
+        </is>
+      </c>
+      <c r="B147">
+        <v>155.2</v>
+      </c>
+      <c r="C147">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>04_21/22</t>
+        </is>
+      </c>
+      <c r="B148">
+        <v>158.4</v>
+      </c>
+      <c r="C148">
+        <v>6.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update links and hyperlinks
</commit_message>
<xml_diff>
--- a/r-fundamentals-5/data/tflSubset.xlsx
+++ b/r-fundamentals-5/data/tflSubset.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2240,10 +2240,10 @@
         </is>
       </c>
       <c r="B145">
-        <v>132.98470079</v>
+        <v>133</v>
       </c>
       <c r="C145">
-        <v>6.149277136</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="146">
@@ -2253,10 +2253,10 @@
         </is>
       </c>
       <c r="B146">
-        <v>146.43823</v>
+        <v>146.5</v>
       </c>
       <c r="C146">
-        <v>6.486115140000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="147">
@@ -2266,10 +2266,10 @@
         </is>
       </c>
       <c r="B147">
-        <v>155.20298203</v>
+        <v>155.2</v>
       </c>
       <c r="C147">
-        <v>7.062506313</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="148">
@@ -2279,10 +2279,10 @@
         </is>
       </c>
       <c r="B148">
-        <v>158.38763834</v>
+        <v>158.4</v>
       </c>
       <c r="C148">
-        <v>6.866115832999999</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="149">
@@ -2292,10 +2292,23 @@
         </is>
       </c>
       <c r="B149">
-        <v>150.07156739</v>
+        <v>150.1</v>
       </c>
       <c r="C149">
-        <v>6.789554679</v>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>06_21/22</t>
+        </is>
+      </c>
+      <c r="B150">
+        <v>173.4</v>
+      </c>
+      <c r="C150">
+        <v>7.100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update intro, R 5 formatting
</commit_message>
<xml_diff>
--- a/r-fundamentals-5/data/tflSubset.xlsx
+++ b/r-fundamentals-5/data/tflSubset.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2467,6 +2467,45 @@
         <v>7.9</v>
       </c>
     </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>06_22/23</t>
+        </is>
+      </c>
+      <c r="B163">
+        <v>211.8</v>
+      </c>
+      <c r="C163">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>07_22/23</t>
+        </is>
+      </c>
+      <c r="B164">
+        <v>234.4</v>
+      </c>
+      <c r="C164">
+        <v>9.199999999999999</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>08_22/23</t>
+        </is>
+      </c>
+      <c r="B165">
+        <v>229.8</v>
+      </c>
+      <c r="C165">
+        <v>9.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>